<commit_message>
remove dummy inputs from quote worksheets
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/HKD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/HKD_YC3MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250" activeTab="6"/>
+    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="3M" sheetId="5" r:id="rId1"/>
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="176">
   <si>
     <t>_Quote</t>
   </si>
@@ -747,6 +747,60 @@
   <si>
     <t>Rate Helpers Selection</t>
   </si>
+  <si>
+    <t>HKD_YC3MRH_1x4F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_2x5F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_3x6F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_4x7F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_5x8F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_6x9F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_7x10F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_8x11F</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H1Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H18M</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H2Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H3Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H4Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H5Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H7Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H10Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H12Y</t>
+  </si>
+  <si>
+    <t>HKD_YC3MRH_QM3H15Y</t>
+  </si>
 </sst>
 </file>
 
@@ -767,7 +821,7 @@
     <numFmt numFmtId="175" formatCode="0.00000%"/>
     <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,6 +942,11 @@
     <font>
       <sz val="8"/>
       <color indexed="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="5"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -1414,7 +1473,7 @@
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
@@ -1848,6 +1907,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="3"/>
@@ -2214,13 +2274,13 @@
         <f>$G$1&amp;"_FRAs.xml"</f>
         <v>HKD_YC3MRH_FRAs.xml</v>
       </c>
-      <c r="H2" s="45" t="e">
+      <c r="H2" s="45">
         <f ca="1">IF(Serialize,_xll.ohObjectSave(H3:H13,SerializationPath&amp;G2,FileOverwrite,,Serialize),"---")</f>
-        <v>#NUM!</v>
+        <v>11</v>
       </c>
       <c r="I2" s="44" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(H2)</f>
-        <v>ohObjectSave - operToVectorImpl: error converting parameter 'ObjectList' to type 'class std::basic_string&lt;char,struct std::char_traits&lt;char&gt;,class std::allocator&lt;char&gt; &gt;' : Unable to convert type 'struct ObjectHandler::empty_property_tag' to type 'class s</v>
+        <v/>
       </c>
       <c r="J2" s="29"/>
     </row>
@@ -2248,13 +2308,13 @@
         <f t="shared" ref="G3:G13" si="2">$G$1&amp;"_"&amp;$C3&amp;$D3</f>
         <v>HKD_YC3MRH_T3F1</v>
       </c>
-      <c r="H3" s="41" t="e">
+      <c r="H3" s="41" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_T3F1#0002</v>
       </c>
       <c r="I3" s="40" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(H3)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDT3F1_Quote'</v>
+        <f>_xll.ohRangeRetrieveError(H3)</f>
+        <v/>
       </c>
       <c r="J3" s="29"/>
     </row>
@@ -2282,13 +2342,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_TOM3F1</v>
       </c>
-      <c r="H4" s="31" t="e">
+      <c r="H4" s="31" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_TOM3F1#0002</v>
       </c>
       <c r="I4" s="39" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(H4)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDTOM3F1_Quote'</v>
+        <f>_xll.ohRangeRetrieveError(H4)</f>
+        <v/>
       </c>
       <c r="J4" s="29"/>
     </row>
@@ -2319,7 +2379,7 @@
       </c>
       <c r="H5" s="36" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1x4F#0001</v>
+        <v>HKD_YC3MRH_1x4F#0002</v>
       </c>
       <c r="I5" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -2354,7 +2414,7 @@
       </c>
       <c r="H6" s="36" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2x5F#0001</v>
+        <v>HKD_YC3MRH_2x5F#0002</v>
       </c>
       <c r="I6" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -2389,7 +2449,7 @@
       </c>
       <c r="H7" s="36" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3x6F#0001</v>
+        <v>HKD_YC3MRH_3x6F#0002</v>
       </c>
       <c r="I7" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -2424,7 +2484,7 @@
       </c>
       <c r="H8" s="36" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4x7F#0001</v>
+        <v>HKD_YC3MRH_4x7F#0002</v>
       </c>
       <c r="I8" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -2459,7 +2519,7 @@
       </c>
       <c r="H9" s="36" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_5x8F#0001</v>
+        <v>HKD_YC3MRH_5x8F#0002</v>
       </c>
       <c r="I9" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -2494,7 +2554,7 @@
       </c>
       <c r="H10" s="36" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_6x9F#0001</v>
+        <v>HKD_YC3MRH_6x9F#0002</v>
       </c>
       <c r="I10" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -2529,7 +2589,7 @@
       </c>
       <c r="H11" s="36" t="str">
         <f>_xll.qlFraRateHelper(G11,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_7x10F#0001</v>
+        <v>HKD_YC3MRH_7x10F#0002</v>
       </c>
       <c r="I11" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -2564,7 +2624,7 @@
       </c>
       <c r="H12" s="36" t="str">
         <f>_xll.qlFraRateHelper(G12,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_8x11F#0001</v>
+        <v>HKD_YC3MRH_8x11F#0002</v>
       </c>
       <c r="I12" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -2599,7 +2659,7 @@
       </c>
       <c r="H13" s="31" t="str">
         <f>_xll.qlFraRateHelper(G13,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_9x12F#0001</v>
+        <v>HKD_YC3MRH_9x12F#0002</v>
       </c>
       <c r="I13" s="30" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -2920,13 +2980,13 @@
         <f>K2&amp;"_Swaps.xml"</f>
         <v>HKD_YC3MRH_Swaps.xml</v>
       </c>
-      <c r="L3" s="45" t="e">
+      <c r="L3" s="45">
         <f ca="1">IF(Serialize,_xll.ohObjectSave(L4:L50,SerializationPath&amp;K3,FileOverwrite,,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M3" s="62" t="e">
+        <v>45</v>
+      </c>
+      <c r="M3" s="62" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L3)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N3" s="61"/>
       <c r="S3" s="85" t="s">
@@ -2962,7 +3022,7 @@
       </c>
       <c r="L4" s="83" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,S4,Currency,T4,U4,V4,W4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H_Hibor3M#0002</v>
+        <v>HKD_YC3MRH_QM3H_Hibor3M#0003</v>
       </c>
       <c r="M4" s="82" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -3040,7 +3100,7 @@
       </c>
       <c r="L6" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H1Y#0001</v>
+        <v>HKD_YC3MRH_QM3H1Y#0002</v>
       </c>
       <c r="M6" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -3092,13 +3152,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H15M</v>
       </c>
-      <c r="L7" s="63" t="e">
+      <c r="L7" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M7" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L7)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H15M#0002</v>
+      </c>
+      <c r="M7" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L7)</f>
+        <v/>
       </c>
       <c r="N7" s="61"/>
       <c r="P7" s="78" t="s">
@@ -3148,7 +3208,7 @@
       </c>
       <c r="L8" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18M#0001</v>
+        <v>HKD_YC3MRH_QM3H18M#0002</v>
       </c>
       <c r="M8" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -3200,13 +3260,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H21M</v>
       </c>
-      <c r="L9" s="63" t="e">
+      <c r="L9" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M9" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L9)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H21M#0002</v>
+      </c>
+      <c r="M9" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L9)</f>
+        <v/>
       </c>
       <c r="N9" s="61"/>
       <c r="P9" s="78" t="s">
@@ -3256,7 +3316,7 @@
       </c>
       <c r="L10" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H2Y#0001</v>
+        <v>HKD_YC3MRH_QM3H2Y#0002</v>
       </c>
       <c r="M10" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -3310,7 +3370,7 @@
       </c>
       <c r="L11" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H3Y#0001</v>
+        <v>HKD_YC3MRH_QM3H3Y#0002</v>
       </c>
       <c r="M11" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -3364,7 +3424,7 @@
       </c>
       <c r="L12" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H4Y#0001</v>
+        <v>HKD_YC3MRH_QM3H4Y#0002</v>
       </c>
       <c r="M12" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -3409,7 +3469,7 @@
       </c>
       <c r="L13" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H5Y#0001</v>
+        <v>HKD_YC3MRH_QM3H5Y#0002</v>
       </c>
       <c r="M13" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -3452,13 +3512,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H6Y</v>
       </c>
-      <c r="L14" s="63" t="e">
+      <c r="L14" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M14" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L14)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H6Y#0002</v>
+      </c>
+      <c r="M14" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L14)</f>
+        <v/>
       </c>
       <c r="N14" s="61"/>
     </row>
@@ -3499,7 +3559,7 @@
       </c>
       <c r="L15" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H7Y#0001</v>
+        <v>HKD_YC3MRH_QM3H7Y#0002</v>
       </c>
       <c r="M15" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -3542,13 +3602,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H8Y</v>
       </c>
-      <c r="L16" s="63" t="e">
+      <c r="L16" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M16" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L16)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H8Y#0002</v>
+      </c>
+      <c r="M16" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L16)</f>
+        <v/>
       </c>
       <c r="N16" s="61"/>
     </row>
@@ -3587,13 +3647,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H9Y</v>
       </c>
-      <c r="L17" s="63" t="e">
+      <c r="L17" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M17" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L17)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H9Y#0002</v>
+      </c>
+      <c r="M17" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L17)</f>
+        <v/>
       </c>
       <c r="N17" s="61"/>
     </row>
@@ -3634,7 +3694,7 @@
       </c>
       <c r="L18" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H10Y#0001</v>
+        <v>HKD_YC3MRH_QM3H10Y#0002</v>
       </c>
       <c r="M18" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -3677,13 +3737,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H11Y</v>
       </c>
-      <c r="L19" s="63" t="e">
+      <c r="L19" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M19" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L19)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H11Y#0002</v>
+      </c>
+      <c r="M19" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L19)</f>
+        <v/>
       </c>
       <c r="N19" s="61"/>
     </row>
@@ -3724,7 +3784,7 @@
       </c>
       <c r="L20" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H12Y#0001</v>
+        <v>HKD_YC3MRH_QM3H12Y#0002</v>
       </c>
       <c r="M20" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -3767,13 +3827,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H13Y</v>
       </c>
-      <c r="L21" s="63" t="e">
+      <c r="L21" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M21" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L21)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H13Y#0002</v>
+      </c>
+      <c r="M21" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L21)</f>
+        <v/>
       </c>
       <c r="N21" s="61"/>
     </row>
@@ -3812,13 +3872,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H14Y</v>
       </c>
-      <c r="L22" s="63" t="e">
+      <c r="L22" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M22" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L22)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H14Y#0002</v>
+      </c>
+      <c r="M22" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L22)</f>
+        <v/>
       </c>
       <c r="N22" s="61"/>
     </row>
@@ -3859,7 +3919,7 @@
       </c>
       <c r="L23" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15Y#0001</v>
+        <v>HKD_YC3MRH_QM3H15Y#0002</v>
       </c>
       <c r="M23" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -3902,13 +3962,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H16Y</v>
       </c>
-      <c r="L24" s="63" t="e">
+      <c r="L24" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M24" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L24)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H16Y#0002</v>
+      </c>
+      <c r="M24" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L24)</f>
+        <v/>
       </c>
       <c r="N24" s="61"/>
     </row>
@@ -3947,13 +4007,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H17Y</v>
       </c>
-      <c r="L25" s="63" t="e">
+      <c r="L25" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M25" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L25)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H17Y#0002</v>
+      </c>
+      <c r="M25" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L25)</f>
+        <v/>
       </c>
       <c r="N25" s="61"/>
     </row>
@@ -3992,13 +4052,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H18Y</v>
       </c>
-      <c r="L26" s="63" t="e">
+      <c r="L26" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M26" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L26)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H18Y#0002</v>
+      </c>
+      <c r="M26" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L26)</f>
+        <v/>
       </c>
       <c r="N26" s="61"/>
     </row>
@@ -4037,13 +4097,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H19Y</v>
       </c>
-      <c r="L27" s="63" t="e">
+      <c r="L27" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M27" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L27)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H19Y#0002</v>
+      </c>
+      <c r="M27" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L27)</f>
+        <v/>
       </c>
       <c r="N27" s="61"/>
     </row>
@@ -4082,13 +4142,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H20Y</v>
       </c>
-      <c r="L28" s="63" t="e">
+      <c r="L28" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M28" s="62" t="e">
-        <f ca="1">_xll.ohRangeRetrieveError(L28)</f>
-        <v>#NUM!</v>
+        <v>HKD_YC3MRH_QM3H20Y#0002</v>
+      </c>
+      <c r="M28" s="62" t="str">
+        <f>_xll.ohRangeRetrieveError(L28)</f>
+        <v/>
       </c>
       <c r="N28" s="61"/>
     </row>
@@ -4129,7 +4189,7 @@
       </c>
       <c r="L29" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21Y#0001</v>
+        <v>HKD_YC3MRH_QM3H21Y#0002</v>
       </c>
       <c r="M29" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -4174,7 +4234,7 @@
       </c>
       <c r="L30" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H22Y#0001</v>
+        <v>HKD_YC3MRH_QM3H22Y#0002</v>
       </c>
       <c r="M30" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -4219,7 +4279,7 @@
       </c>
       <c r="L31" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H23Y#0001</v>
+        <v>HKD_YC3MRH_QM3H23Y#0002</v>
       </c>
       <c r="M31" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -4264,7 +4324,7 @@
       </c>
       <c r="L32" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H24Y#0001</v>
+        <v>HKD_YC3MRH_QM3H24Y#0002</v>
       </c>
       <c r="M32" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -4309,7 +4369,7 @@
       </c>
       <c r="L33" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H25Y#0001</v>
+        <v>HKD_YC3MRH_QM3H25Y#0002</v>
       </c>
       <c r="M33" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -4354,7 +4414,7 @@
       </c>
       <c r="L34" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H26Y#0001</v>
+        <v>HKD_YC3MRH_QM3H26Y#0002</v>
       </c>
       <c r="M34" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -4399,7 +4459,7 @@
       </c>
       <c r="L35" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H27Y#0001</v>
+        <v>HKD_YC3MRH_QM3H27Y#0002</v>
       </c>
       <c r="M35" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -4444,7 +4504,7 @@
       </c>
       <c r="L36" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H28Y#0001</v>
+        <v>HKD_YC3MRH_QM3H28Y#0002</v>
       </c>
       <c r="M36" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -4489,7 +4549,7 @@
       </c>
       <c r="L37" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H29Y#0001</v>
+        <v>HKD_YC3MRH_QM3H29Y#0002</v>
       </c>
       <c r="M37" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -4534,7 +4594,7 @@
       </c>
       <c r="L38" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H30Y#0001</v>
+        <v>HKD_YC3MRH_QM3H30Y#0002</v>
       </c>
       <c r="M38" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -4579,7 +4639,7 @@
       </c>
       <c r="L39" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H35Y#0001</v>
+        <v>HKD_YC3MRH_QM3H35Y#0002</v>
       </c>
       <c r="M39" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -4624,7 +4684,7 @@
       </c>
       <c r="L40" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H40Y#0001</v>
+        <v>HKD_YC3MRH_QM3H40Y#0002</v>
       </c>
       <c r="M40" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -4669,7 +4729,7 @@
       </c>
       <c r="L41" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H50Y#0001</v>
+        <v>HKD_YC3MRH_QM3H50Y#0002</v>
       </c>
       <c r="M41" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -4714,7 +4774,7 @@
       </c>
       <c r="L42" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H60Y#0001</v>
+        <v>HKD_YC3MRH_QM3H60Y#0002</v>
       </c>
       <c r="M42" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -4772,7 +4832,7 @@
       </c>
       <c r="L44" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S12#0001</v>
+        <v>HKD_YC3MRH_1S12#0002</v>
       </c>
       <c r="M44" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -4815,7 +4875,7 @@
       </c>
       <c r="L45" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2S12#0001</v>
+        <v>HKD_YC3MRH_2S12#0002</v>
       </c>
       <c r="M45" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -4860,7 +4920,7 @@
       </c>
       <c r="L46" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3S12#0001</v>
+        <v>HKD_YC3MRH_3S12#0002</v>
       </c>
       <c r="M46" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -4905,7 +4965,7 @@
       </c>
       <c r="L47" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4S12#0001</v>
+        <v>HKD_YC3MRH_4S12#0002</v>
       </c>
       <c r="M47" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -4950,7 +5010,7 @@
       </c>
       <c r="L48" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S24#0001</v>
+        <v>HKD_YC3MRH_1S24#0002</v>
       </c>
       <c r="M48" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -4995,7 +5055,7 @@
       </c>
       <c r="L49" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2S24#0001</v>
+        <v>HKD_YC3MRH_2S24#0002</v>
       </c>
       <c r="M49" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -5040,7 +5100,7 @@
       </c>
       <c r="L50" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S36#0001</v>
+        <v>HKD_YC3MRH_1S36#0002</v>
       </c>
       <c r="M50" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -6007,9 +6067,9 @@
         <f t="shared" si="0"/>
         <v>HKD_YC3MRH_T3F1</v>
       </c>
-      <c r="F16" s="155" t="e">
+      <c r="F16" s="155" t="str">
         <f>_xll.ohObjectPropertyValues(E16,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDT3F1_Quote</v>
       </c>
       <c r="G16" s="154" t="e">
         <f>_xll.qlRateHelperQuoteValue($E16,Trigger)</f>
@@ -6025,13 +6085,13 @@
       <c r="K16" s="153">
         <v>1</v>
       </c>
-      <c r="L16" s="152" t="e">
+      <c r="L16" s="152">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M16" s="151" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M16" s="151">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41689</v>
       </c>
       <c r="P16" s="134" t="e">
         <v>#NUM!</v>
@@ -6052,9 +6112,9 @@
         <f t="shared" si="0"/>
         <v>HKD_YC3MRH_TOM3F1</v>
       </c>
-      <c r="F17" s="140" t="e">
+      <c r="F17" s="140" t="str">
         <f>_xll.ohObjectPropertyValues(E17,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDTOM3F1_Quote</v>
       </c>
       <c r="G17" s="139" t="e">
         <f>_xll.qlRateHelperQuoteValue($E17,Trigger)</f>
@@ -6070,13 +6130,13 @@
       <c r="K17" s="138">
         <v>1</v>
       </c>
-      <c r="L17" s="137" t="e">
+      <c r="L17" s="137">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M17" s="136" t="e">
+        <v>41598</v>
+      </c>
+      <c r="M17" s="136">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41690</v>
       </c>
       <c r="P17" s="134" t="e">
         <v>#NUM!</v>
@@ -6101,9 +6161,9 @@
         <f>_xll.ohObjectPropertyValues(E18,"Rate")</f>
         <v>HKD1x4F_Quote</v>
       </c>
-      <c r="G18" s="146">
+      <c r="G18" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H18" s="146"/>
       <c r="I18" s="145" t="b">
@@ -6146,9 +6206,9 @@
         <f>_xll.ohObjectPropertyValues(E19,"Rate")</f>
         <v>HKD2x5F_Quote</v>
       </c>
-      <c r="G19" s="146">
+      <c r="G19" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H19" s="146"/>
       <c r="I19" s="145" t="b">
@@ -6191,9 +6251,9 @@
         <f>_xll.ohObjectPropertyValues(E20,"Rate")</f>
         <v>HKD3x6F_Quote</v>
       </c>
-      <c r="G20" s="146">
+      <c r="G20" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H20" s="146"/>
       <c r="I20" s="145" t="b">
@@ -6236,9 +6296,9 @@
         <f>_xll.ohObjectPropertyValues(E21,"Rate")</f>
         <v>HKD4x7F_Quote</v>
       </c>
-      <c r="G21" s="146">
+      <c r="G21" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>4.3E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H21" s="146"/>
       <c r="I21" s="145" t="b">
@@ -6281,9 +6341,9 @@
         <f>_xll.ohObjectPropertyValues(E22,"Rate")</f>
         <v>HKD5x8F_Quote</v>
       </c>
-      <c r="G22" s="146">
+      <c r="G22" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>4.4000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H22" s="146"/>
       <c r="I22" s="145" t="b">
@@ -6326,9 +6386,9 @@
         <f>_xll.ohObjectPropertyValues(E23,"Rate")</f>
         <v>HKD6x9F_Quote</v>
       </c>
-      <c r="G23" s="146">
+      <c r="G23" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>4.4999999999999997E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H23" s="146"/>
       <c r="I23" s="145" t="b">
@@ -6371,9 +6431,9 @@
         <f>_xll.ohObjectPropertyValues(E24,"Rate")</f>
         <v>HKD7x10F_Quote</v>
       </c>
-      <c r="G24" s="146">
+      <c r="G24" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E24,Trigger)</f>
-        <v>4.7000000000000002E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H24" s="146"/>
       <c r="I24" s="145" t="b">
@@ -6416,9 +6476,9 @@
         <f>_xll.ohObjectPropertyValues(E25,"Rate")</f>
         <v>HKD8x11F_Quote</v>
       </c>
-      <c r="G25" s="146">
+      <c r="G25" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E25,Trigger)</f>
-        <v>4.7999999999999996E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H25" s="146"/>
       <c r="I25" s="145" t="b">
@@ -6461,9 +6521,9 @@
         <f>_xll.ohObjectPropertyValues(E26,"Rate")</f>
         <v>HKD9x12F_Quote</v>
       </c>
-      <c r="G26" s="146">
+      <c r="G26" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E26,Trigger)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H26" s="146"/>
       <c r="I26" s="145" t="b">
@@ -9585,9 +9645,9 @@
         <f>_xll.ohObjectPropertyValues(E96,"Rate")</f>
         <v>HKDQM3H1Y_Quote</v>
       </c>
-      <c r="G96" s="146">
+      <c r="G96" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E96,Trigger)</f>
-        <v>4.4000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H96" s="146">
         <f>_xll.qlSwapRateHelperSpread($E96,Trigger)</f>
@@ -9595,7 +9655,7 @@
       </c>
       <c r="I96" s="145" t="b">
         <f t="shared" ref="I96:I132" si="8">IF(ISERROR(G96),FALSE,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J96" s="145">
         <v>50</v>
@@ -9632,17 +9692,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_QM3H15M</v>
       </c>
-      <c r="F97" s="147" t="e">
+      <c r="F97" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E97,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H15M_Quote</v>
       </c>
       <c r="G97" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E97,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H97" s="146" t="e">
+      <c r="H97" s="146">
         <f>_xll.qlSwapRateHelperSpread($E97,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I97" s="145" t="b">
         <f t="shared" si="8"/>
@@ -9654,13 +9714,13 @@
       <c r="K97" s="145">
         <v>1</v>
       </c>
-      <c r="L97" s="144" t="e">
+      <c r="L97" s="144">
         <f>_xll.qlRateHelperEarliestDate($E97,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M97" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M97" s="143">
         <f>_xll.qlRateHelperLatestDate($E97,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42054</v>
       </c>
       <c r="O97" s="150" t="e">
         <f t="shared" si="9"/>
@@ -9687,9 +9747,9 @@
         <f>_xll.ohObjectPropertyValues(E98,"Rate")</f>
         <v>HKDQM3H18M_Quote</v>
       </c>
-      <c r="G98" s="146">
+      <c r="G98" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E98,Trigger)</f>
-        <v>4.7999999999999996E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H98" s="146">
         <f>_xll.qlSwapRateHelperSpread($E98,Trigger)</f>
@@ -9697,7 +9757,7 @@
       </c>
       <c r="I98" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98" s="145">
         <v>50</v>
@@ -9734,17 +9794,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H21M</v>
       </c>
-      <c r="F99" s="147" t="e">
+      <c r="F99" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E99,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H21M_Quote</v>
       </c>
       <c r="G99" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E99,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H99" s="146" t="e">
+      <c r="H99" s="146">
         <f>_xll.qlSwapRateHelperSpread($E99,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I99" s="145" t="b">
         <f t="shared" si="8"/>
@@ -9756,13 +9816,13 @@
       <c r="K99" s="145">
         <v>1</v>
       </c>
-      <c r="L99" s="144" t="e">
+      <c r="L99" s="144">
         <f>_xll.qlRateHelperEarliestDate($E99,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M99" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M99" s="143">
         <f>_xll.qlRateHelperLatestDate($E99,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42235</v>
       </c>
       <c r="O99" s="150" t="e">
         <f t="shared" si="9"/>
@@ -9789,9 +9849,9 @@
         <f>_xll.ohObjectPropertyValues(E100,"Rate")</f>
         <v>HKDQM3H2Y_Quote</v>
       </c>
-      <c r="G100" s="146">
+      <c r="G100" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E100,Trigger)</f>
-        <v>5.4000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H100" s="146">
         <f>_xll.qlSwapRateHelperSpread($E100,Trigger)</f>
@@ -9799,7 +9859,7 @@
       </c>
       <c r="I100" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J100" s="145">
         <v>50</v>
@@ -9840,9 +9900,9 @@
         <f>_xll.ohObjectPropertyValues(E101,"Rate")</f>
         <v>HKDQM3H3Y_Quote</v>
       </c>
-      <c r="G101" s="146">
+      <c r="G101" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E101,Trigger)</f>
-        <v>7.7000000000000002E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="H101" s="146">
         <f>_xll.qlSwapRateHelperSpread($E101,Trigger)</f>
@@ -9850,7 +9910,7 @@
       </c>
       <c r="I101" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J101" s="145">
         <v>50</v>
@@ -9891,9 +9951,9 @@
         <f>_xll.ohObjectPropertyValues(E102,"Rate")</f>
         <v>HKDQM3H4Y_Quote</v>
       </c>
-      <c r="G102" s="146">
+      <c r="G102" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E102,Trigger)</f>
-        <v>1.09E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="H102" s="146">
         <f>_xll.qlSwapRateHelperSpread($E102,Trigger)</f>
@@ -9901,7 +9961,7 @@
       </c>
       <c r="I102" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J102" s="145">
         <v>50</v>
@@ -9942,9 +10002,9 @@
         <f>_xll.ohObjectPropertyValues(E103,"Rate")</f>
         <v>HKDQM3H5Y_Quote</v>
       </c>
-      <c r="G103" s="146">
+      <c r="G103" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E103,Trigger)</f>
-        <v>1.41E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="H103" s="146">
         <f>_xll.qlSwapRateHelperSpread($E103,Trigger)</f>
@@ -9952,7 +10012,7 @@
       </c>
       <c r="I103" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J103" s="145">
         <v>50</v>
@@ -9989,17 +10049,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H6Y</v>
       </c>
-      <c r="F104" s="147" t="e">
+      <c r="F104" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E104,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H6Y_Quote</v>
       </c>
       <c r="G104" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E104,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H104" s="146" t="e">
+      <c r="H104" s="146">
         <f>_xll.qlSwapRateHelperSpread($E104,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I104" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10011,13 +10071,13 @@
       <c r="K104" s="145">
         <v>1</v>
       </c>
-      <c r="L104" s="144" t="e">
+      <c r="L104" s="144">
         <f>_xll.qlRateHelperEarliestDate($E104,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M104" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M104" s="143">
         <f>_xll.qlRateHelperLatestDate($E104,Trigger)</f>
-        <v>#NUM!</v>
+        <v>43788</v>
       </c>
       <c r="O104" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10044,9 +10104,9 @@
         <f>_xll.ohObjectPropertyValues(E105,"Rate")</f>
         <v>HKDQM3H7Y_Quote</v>
       </c>
-      <c r="G105" s="146">
+      <c r="G105" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E105,Trigger)</f>
-        <v>1.95E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="H105" s="146">
         <f>_xll.qlSwapRateHelperSpread($E105,Trigger)</f>
@@ -10054,7 +10114,7 @@
       </c>
       <c r="I105" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J105" s="145">
         <v>50</v>
@@ -10091,17 +10151,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H8Y</v>
       </c>
-      <c r="F106" s="147" t="e">
+      <c r="F106" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E106,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H8Y_Quote</v>
       </c>
       <c r="G106" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E106,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H106" s="146" t="e">
+      <c r="H106" s="146">
         <f>_xll.qlSwapRateHelperSpread($E106,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I106" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10113,13 +10173,13 @@
       <c r="K106" s="145">
         <v>1</v>
       </c>
-      <c r="L106" s="144" t="e">
+      <c r="L106" s="144">
         <f>_xll.qlRateHelperEarliestDate($E106,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M106" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M106" s="143">
         <f>_xll.qlRateHelperLatestDate($E106,Trigger)</f>
-        <v>#NUM!</v>
+        <v>44519</v>
       </c>
       <c r="O106" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10142,17 +10202,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H9Y</v>
       </c>
-      <c r="F107" s="147" t="e">
+      <c r="F107" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E107,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H9Y_Quote</v>
       </c>
       <c r="G107" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E107,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H107" s="146" t="e">
+      <c r="H107" s="146">
         <f>_xll.qlSwapRateHelperSpread($E107,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I107" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10164,13 +10224,13 @@
       <c r="K107" s="145">
         <v>1</v>
       </c>
-      <c r="L107" s="144" t="e">
+      <c r="L107" s="144">
         <f>_xll.qlRateHelperEarliestDate($E107,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M107" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M107" s="143">
         <f>_xll.qlRateHelperLatestDate($E107,Trigger)</f>
-        <v>#NUM!</v>
+        <v>44886</v>
       </c>
       <c r="O107" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10197,9 +10257,9 @@
         <f>_xll.ohObjectPropertyValues(E108,"Rate")</f>
         <v>HKDQM3H10Y_Quote</v>
       </c>
-      <c r="G108" s="146">
+      <c r="G108" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E108,Trigger)</f>
-        <v>2.4500000000000001E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="H108" s="146">
         <f>_xll.qlSwapRateHelperSpread($E108,Trigger)</f>
@@ -10207,7 +10267,7 @@
       </c>
       <c r="I108" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J108" s="145">
         <v>50</v>
@@ -10244,17 +10304,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H11Y</v>
       </c>
-      <c r="F109" s="147" t="e">
+      <c r="F109" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E109,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H11Y_Quote</v>
       </c>
       <c r="G109" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E109,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H109" s="146" t="e">
+      <c r="H109" s="146">
         <f>_xll.qlSwapRateHelperSpread($E109,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I109" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10266,13 +10326,13 @@
       <c r="K109" s="145">
         <v>1</v>
       </c>
-      <c r="L109" s="144" t="e">
+      <c r="L109" s="144">
         <f>_xll.qlRateHelperEarliestDate($E109,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M109" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M109" s="143">
         <f>_xll.qlRateHelperLatestDate($E109,Trigger)</f>
-        <v>#NUM!</v>
+        <v>45615</v>
       </c>
       <c r="O109" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10299,9 +10359,9 @@
         <f>_xll.ohObjectPropertyValues(E110,"Rate")</f>
         <v>HKDQM3H12Y_Quote</v>
       </c>
-      <c r="G110" s="146">
+      <c r="G110" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E110,Trigger)</f>
-        <v>2.6100000000000002E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="H110" s="146">
         <f>_xll.qlSwapRateHelperSpread($E110,Trigger)</f>
@@ -10309,7 +10369,7 @@
       </c>
       <c r="I110" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J110" s="145">
         <v>50</v>
@@ -10346,17 +10406,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H13Y</v>
       </c>
-      <c r="F111" s="147" t="e">
+      <c r="F111" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E111,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H13Y_Quote</v>
       </c>
       <c r="G111" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E111,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H111" s="146" t="e">
+      <c r="H111" s="146">
         <f>_xll.qlSwapRateHelperSpread($E111,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I111" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10368,13 +10428,13 @@
       <c r="K111" s="145">
         <v>1</v>
       </c>
-      <c r="L111" s="144" t="e">
+      <c r="L111" s="144">
         <f>_xll.qlRateHelperEarliestDate($E111,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M111" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M111" s="143">
         <f>_xll.qlRateHelperLatestDate($E111,Trigger)</f>
-        <v>#NUM!</v>
+        <v>46345</v>
       </c>
       <c r="O111" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10397,17 +10457,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H14Y</v>
       </c>
-      <c r="F112" s="147" t="e">
+      <c r="F112" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E112,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H14Y_Quote</v>
       </c>
       <c r="G112" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E112,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H112" s="146" t="e">
+      <c r="H112" s="146">
         <f>_xll.qlSwapRateHelperSpread($E112,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I112" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10419,13 +10479,13 @@
       <c r="K112" s="145">
         <v>1</v>
       </c>
-      <c r="L112" s="144" t="e">
+      <c r="L112" s="144">
         <f>_xll.qlRateHelperEarliestDate($E112,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M112" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M112" s="143">
         <f>_xll.qlRateHelperLatestDate($E112,Trigger)</f>
-        <v>#NUM!</v>
+        <v>46710</v>
       </c>
       <c r="O112" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10452,9 +10512,9 @@
         <f>_xll.ohObjectPropertyValues(E113,"Rate")</f>
         <v>HKDQM3H15Y_Quote</v>
       </c>
-      <c r="G113" s="146">
+      <c r="G113" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E113,Trigger)</f>
-        <v>2.7199999999999998E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="H113" s="146">
         <f>_xll.qlSwapRateHelperSpread($E113,Trigger)</f>
@@ -10462,7 +10522,7 @@
       </c>
       <c r="I113" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J113" s="145">
         <v>50</v>
@@ -10499,17 +10559,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H16Y</v>
       </c>
-      <c r="F114" s="147" t="e">
+      <c r="F114" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E114,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H16Y_Quote</v>
       </c>
       <c r="G114" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E114,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H114" s="146" t="e">
+      <c r="H114" s="146">
         <f>_xll.qlSwapRateHelperSpread($E114,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I114" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10521,13 +10581,13 @@
       <c r="K114" s="145">
         <v>1</v>
       </c>
-      <c r="L114" s="144" t="e">
+      <c r="L114" s="144">
         <f>_xll.qlRateHelperEarliestDate($E114,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M114" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M114" s="143">
         <f>_xll.qlRateHelperLatestDate($E114,Trigger)</f>
-        <v>#NUM!</v>
+        <v>47441</v>
       </c>
       <c r="O114" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10550,17 +10610,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H17Y</v>
       </c>
-      <c r="F115" s="147" t="e">
+      <c r="F115" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E115,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H17Y_Quote</v>
       </c>
       <c r="G115" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E115,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H115" s="146" t="e">
+      <c r="H115" s="146">
         <f>_xll.qlSwapRateHelperSpread($E115,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I115" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10572,13 +10632,13 @@
       <c r="K115" s="145">
         <v>1</v>
       </c>
-      <c r="L115" s="144" t="e">
+      <c r="L115" s="144">
         <f>_xll.qlRateHelperEarliestDate($E115,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M115" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M115" s="143">
         <f>_xll.qlRateHelperLatestDate($E115,Trigger)</f>
-        <v>#NUM!</v>
+        <v>47806</v>
       </c>
       <c r="O115" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10601,17 +10661,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H18Y</v>
       </c>
-      <c r="F116" s="147" t="e">
+      <c r="F116" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E116,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H18Y_Quote</v>
       </c>
       <c r="G116" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E116,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H116" s="146" t="e">
+      <c r="H116" s="146">
         <f>_xll.qlSwapRateHelperSpread($E116,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I116" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10623,13 +10683,13 @@
       <c r="K116" s="145">
         <v>1</v>
       </c>
-      <c r="L116" s="144" t="e">
+      <c r="L116" s="144">
         <f>_xll.qlRateHelperEarliestDate($E116,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M116" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M116" s="143">
         <f>_xll.qlRateHelperLatestDate($E116,Trigger)</f>
-        <v>#NUM!</v>
+        <v>48171</v>
       </c>
       <c r="O116" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10652,17 +10712,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H19Y</v>
       </c>
-      <c r="F117" s="147" t="e">
+      <c r="F117" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E117,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H19Y_Quote</v>
       </c>
       <c r="G117" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E117,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H117" s="146" t="e">
+      <c r="H117" s="146">
         <f>_xll.qlSwapRateHelperSpread($E117,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I117" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10674,13 +10734,13 @@
       <c r="K117" s="145">
         <v>1</v>
       </c>
-      <c r="L117" s="144" t="e">
+      <c r="L117" s="144">
         <f>_xll.qlRateHelperEarliestDate($E117,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M117" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M117" s="143">
         <f>_xll.qlRateHelperLatestDate($E117,Trigger)</f>
-        <v>#NUM!</v>
+        <v>48537</v>
       </c>
       <c r="O117" s="150" t="e">
         <f t="shared" si="9"/>
@@ -10703,17 +10763,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H20Y</v>
       </c>
-      <c r="F118" s="147" t="e">
+      <c r="F118" s="147" t="str">
         <f>_xll.ohObjectPropertyValues(E118,"Rate")</f>
-        <v>#NUM!</v>
+        <v>HKDQM3H20Y_Quote</v>
       </c>
       <c r="G118" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E118,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H118" s="146" t="e">
+      <c r="H118" s="146">
         <f>_xll.qlSwapRateHelperSpread($E118,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I118" s="145" t="b">
         <f t="shared" si="8"/>
@@ -10725,13 +10785,13 @@
       <c r="K118" s="145">
         <v>1</v>
       </c>
-      <c r="L118" s="144" t="e">
+      <c r="L118" s="144">
         <f>_xll.qlRateHelperEarliestDate($E118,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M118" s="143" t="e">
+        <v>41597</v>
+      </c>
+      <c r="M118" s="143">
         <f>_xll.qlRateHelperLatestDate($E118,Trigger)</f>
-        <v>#NUM!</v>
+        <v>48904</v>
       </c>
       <c r="O118" s="150" t="e">
         <f t="shared" si="9"/>
@@ -13169,15 +13229,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.85546875" style="134" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="134" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="134" customWidth="1"/>
+    <col min="3" max="3" width="13" style="134" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" style="135" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8" style="135" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="17.28515625" style="135" bestFit="1" customWidth="1"/>
@@ -13203,9 +13263,9 @@
       <c r="H1" s="183" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="165">
+      <c r="I1" s="165" t="e">
         <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -13215,13 +13275,16 @@
       <c r="B2" s="181">
         <v>0</v>
       </c>
+      <c r="C2" s="197" t="s">
+        <v>158</v>
+      </c>
       <c r="D2" s="173" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
         <v>HKD_YC3MRH_1x4F</v>
       </c>
-      <c r="E2" s="172">
+      <c r="E2" s="172" t="e">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F2" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -13235,8 +13298,8 @@
         <f>_xll.qlRateHelperLatestDate($D2)</f>
         <v>41717</v>
       </c>
-      <c r="I2" s="165">
-        <v>0.99865364000379186</v>
+      <c r="I2" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -13246,12 +13309,15 @@
       <c r="B3" s="180">
         <v>0</v>
       </c>
+      <c r="C3" s="197" t="s">
+        <v>159</v>
+      </c>
       <c r="D3" s="173" t="str">
         <v>HKD_YC3MRH_2x5F</v>
       </c>
-      <c r="E3" s="172">
+      <c r="E3" s="172" t="e">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F3" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -13265,8 +13331,8 @@
         <f>_xll.qlRateHelperLatestDate($D3)</f>
         <v>41751</v>
       </c>
-      <c r="I3" s="165">
-        <v>0.99827251130700834</v>
+      <c r="I3" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -13276,12 +13342,15 @@
       <c r="B4" s="180">
         <v>0</v>
       </c>
+      <c r="C4" s="197" t="s">
+        <v>160</v>
+      </c>
       <c r="D4" s="173" t="str">
         <v>HKD_YC3MRH_3x6F</v>
       </c>
-      <c r="E4" s="172">
+      <c r="E4" s="172" t="e">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>4.1000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F4" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -13295,8 +13364,8 @@
         <f>_xll.qlRateHelperLatestDate($D4)</f>
         <v>41778</v>
       </c>
-      <c r="I4" s="165">
-        <v>0.9979699290571088</v>
+      <c r="I4" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -13306,12 +13375,15 @@
       <c r="B5" s="179" t="s">
         <v>150</v>
       </c>
+      <c r="C5" s="197" t="s">
+        <v>161</v>
+      </c>
       <c r="D5" s="173" t="str">
         <v>HKD_YC3MRH_4x7F</v>
       </c>
-      <c r="E5" s="172">
+      <c r="E5" s="172" t="e">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>4.3E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F5" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -13325,8 +13397,8 @@
         <f>_xll.qlRateHelperLatestDate($D5)</f>
         <v>41809</v>
       </c>
-      <c r="I5" s="165">
-        <v>0.99757243546815444</v>
+      <c r="I5" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -13337,12 +13409,15 @@
         <f>_xll.ohRangeRetrieveError(Selected!D2)</f>
         <v/>
       </c>
+      <c r="C6" s="197" t="s">
+        <v>162</v>
+      </c>
       <c r="D6" s="173" t="str">
         <v>HKD_YC3MRH_5x8F</v>
       </c>
-      <c r="E6" s="172">
+      <c r="E6" s="172" t="e">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>4.4000000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F6" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -13356,25 +13431,28 @@
         <f>_xll.qlRateHelperLatestDate($D6)</f>
         <v>41842</v>
       </c>
-      <c r="I6" s="165">
-        <v>0.99717862002060087</v>
+      <c r="I6" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="176" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_RateHelpersSelected#0001</v>
+        <v>HKD_YC3MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="175" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
+      <c r="C7" s="197" t="s">
+        <v>163</v>
+      </c>
       <c r="D7" s="173" t="str">
         <v>HKD_YC3MRH_6x9F</v>
       </c>
-      <c r="E7" s="172">
+      <c r="E7" s="172" t="e">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>4.4999999999999997E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F7" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -13388,17 +13466,20 @@
         <f>_xll.qlRateHelperLatestDate($D7)</f>
         <v>41870</v>
       </c>
-      <c r="I7" s="165">
-        <v>0.99683926753185581</v>
+      <c r="I7" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C8" s="197" t="s">
+        <v>164</v>
+      </c>
       <c r="D8" s="173" t="str">
         <v>HKD_YC3MRH_7x10F</v>
       </c>
-      <c r="E8" s="172">
+      <c r="E8" s="172" t="e">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>4.7000000000000002E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F8" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -13412,17 +13493,20 @@
         <f>_xll.qlRateHelperLatestDate($D8)</f>
         <v>41901</v>
       </c>
-      <c r="I8" s="165">
-        <v>0.99639205211643067</v>
+      <c r="I8" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="197" t="s">
+        <v>165</v>
+      </c>
       <c r="D9" s="173" t="str">
         <v>HKD_YC3MRH_8x11F</v>
       </c>
-      <c r="E9" s="172">
+      <c r="E9" s="172" t="e">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>4.7999999999999996E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F9" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -13436,253 +13520,283 @@
         <f>_xll.qlRateHelperLatestDate($D9)</f>
         <v>41933</v>
       </c>
-      <c r="I9" s="165">
-        <v>0.99598562164313242</v>
+      <c r="I9" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="197" t="s">
+        <v>166</v>
+      </c>
       <c r="D10" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H1Y</v>
-      </c>
-      <c r="E10" s="172">
+        <v>HKD_YC3MRH_9x12F</v>
+      </c>
+      <c r="E10" s="172" t="e">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="F10" s="172">
+        <v>#NUM!</v>
+      </c>
+      <c r="F10" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
-        <v>0</v>
+        <v>--</v>
       </c>
       <c r="G10" s="171">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41597</v>
+        <v>41870</v>
       </c>
       <c r="H10" s="170">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
         <v>41962</v>
       </c>
-      <c r="I10" s="165">
-        <v>0.99561169515438841</v>
+      <c r="I10" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H18M</v>
-      </c>
-      <c r="E11" s="172">
+      <c r="C11" s="197" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E11" s="172" t="e">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="F11" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F11" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="171">
+        <v>--</v>
+      </c>
+      <c r="G11" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41597</v>
-      </c>
-      <c r="H11" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42143</v>
-      </c>
-      <c r="I11" s="165">
-        <v>0.99284777808043889</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I11" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="174"/>
-      <c r="D12" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H2Y</v>
-      </c>
-      <c r="E12" s="172">
+      <c r="C12" s="197" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E12" s="172" t="e">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="F12" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F12" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="171">
+        <v>--</v>
+      </c>
+      <c r="G12" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41597</v>
-      </c>
-      <c r="H12" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H12" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42327</v>
-      </c>
-      <c r="I12" s="165">
-        <v>0.98925812337415742</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I12" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="174"/>
-      <c r="D13" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H3Y</v>
-      </c>
-      <c r="E13" s="172">
+      <c r="C13" s="197" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E13" s="172" t="e">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>7.7000000000000002E-3</v>
-      </c>
-      <c r="F13" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="171">
+        <v>--</v>
+      </c>
+      <c r="G13" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41597</v>
-      </c>
-      <c r="H13" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H13" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42695</v>
-      </c>
-      <c r="I13" s="165">
-        <v>0.97705845058217056</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I13" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D14" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H4Y</v>
-      </c>
-      <c r="E14" s="172">
+      <c r="C14" s="197" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E14" s="172" t="e">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>1.09E-2</v>
-      </c>
-      <c r="F14" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="171">
+        <v>--</v>
+      </c>
+      <c r="G14" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41597</v>
-      </c>
-      <c r="H14" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H14" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>43059</v>
-      </c>
-      <c r="I14" s="165">
-        <v>0.95703325949529394</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I14" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H5Y</v>
-      </c>
-      <c r="E15" s="172">
+      <c r="C15" s="197" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E15" s="172" t="e">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>1.41E-2</v>
-      </c>
-      <c r="F15" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F15" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="171">
+        <v>--</v>
+      </c>
+      <c r="G15" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41597</v>
-      </c>
-      <c r="H15" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H15" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>43423</v>
-      </c>
-      <c r="I15" s="165">
-        <v>0.93118294061173668</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I15" s="165" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D16" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H7Y</v>
-      </c>
-      <c r="E16" s="172">
+      <c r="C16" s="197" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E16" s="172" t="e">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.95E-2</v>
-      </c>
-      <c r="F16" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F16" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="171">
+        <v>--</v>
+      </c>
+      <c r="G16" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41597</v>
-      </c>
-      <c r="H16" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>44154</v>
-      </c>
-      <c r="I16" s="165">
-        <v>0.869791904909194</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D17" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H10Y</v>
-      </c>
-      <c r="E17" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I16" s="165" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C17" s="197" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E17" s="172" t="e">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>2.4500000000000001E-2</v>
-      </c>
-      <c r="F17" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F17" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="171">
+        <v>--</v>
+      </c>
+      <c r="G17" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41597</v>
-      </c>
-      <c r="H17" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H17" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>45250</v>
-      </c>
-      <c r="I17" s="165">
-        <v>0.77619760049330866</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D18" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H12Y</v>
-      </c>
-      <c r="E18" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I17" s="165" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C18" s="197" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E18" s="172" t="e">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>2.6100000000000002E-2</v>
-      </c>
-      <c r="F18" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="171">
+        <v>--</v>
+      </c>
+      <c r="G18" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41597</v>
-      </c>
-      <c r="H18" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H18" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>45980</v>
-      </c>
-      <c r="I18" s="165">
-        <v>0.72266935831338064</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D19" s="173" t="str">
-        <v>HKD_YC3MRH_QM3H15Y</v>
-      </c>
-      <c r="E19" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="165" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="197" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" s="173" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E19" s="172" t="e">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>2.7199999999999998E-2</v>
-      </c>
-      <c r="F19" s="172">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="171">
+        <v>--</v>
+      </c>
+      <c r="G19" s="171" t="e">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41597</v>
-      </c>
-      <c r="H19" s="170">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H19" s="170" t="e">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>47077</v>
-      </c>
-      <c r="I19" s="165">
-        <v>0.65497637364458239</v>
-      </c>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" s="165" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D20" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13703,10 +13817,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I20" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D21" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13727,10 +13841,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I21" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D22" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13751,10 +13865,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I22" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D23" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13775,10 +13889,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I23" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D24" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13799,10 +13913,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I24" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D25" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13823,10 +13937,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I25" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D26" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13847,10 +13961,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I26" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D27" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13871,10 +13985,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I27" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D28" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13895,10 +14009,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I28" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D29" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13919,10 +14033,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I29" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D30" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13943,10 +14057,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I30" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D31" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13967,10 +14081,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="I31" s="165" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.2">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D32" s="173" t="e">
         <v>#N/A</v>
       </c>
@@ -13991,7 +14105,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I32" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.2">
@@ -14015,7 +14129,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I33" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.2">
@@ -14039,7 +14153,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I34" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.2">
@@ -14063,7 +14177,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I35" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.2">
@@ -14087,7 +14201,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I36" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.2">
@@ -14111,7 +14225,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I37" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.2">
@@ -14135,7 +14249,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I38" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.2">
@@ -14159,7 +14273,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I39" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.2">
@@ -14183,7 +14297,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I40" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.2">
@@ -14207,7 +14321,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I41" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.2">
@@ -14231,7 +14345,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I42" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.2">
@@ -14255,7 +14369,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I43" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.2">
@@ -14279,7 +14393,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I44" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.2">
@@ -14303,7 +14417,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I45" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.2">
@@ -14327,7 +14441,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I46" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.2">
@@ -14351,7 +14465,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I47" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.2">
@@ -14375,7 +14489,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I48" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.2">
@@ -14399,7 +14513,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I49" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.2">
@@ -14423,7 +14537,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I50" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.2">
@@ -14447,7 +14561,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I51" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.2">
@@ -14471,7 +14585,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I52" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
@@ -14495,7 +14609,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I53" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
@@ -14519,7 +14633,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I54" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="55" spans="4:9" x14ac:dyDescent="0.2">
@@ -14543,7 +14657,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I55" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="56" spans="4:9" x14ac:dyDescent="0.2">
@@ -14567,7 +14681,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I56" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.2">
@@ -14591,7 +14705,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I57" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.2">
@@ -14615,7 +14729,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I58" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="59" spans="4:9" x14ac:dyDescent="0.2">
@@ -14639,7 +14753,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="60" spans="4:9" x14ac:dyDescent="0.2">
@@ -14663,7 +14777,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I60" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.2">
@@ -14687,7 +14801,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I61" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="62" spans="4:9" x14ac:dyDescent="0.2">
@@ -14711,7 +14825,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I62" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.2">
@@ -14735,7 +14849,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I63" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.2">
@@ -14759,7 +14873,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I64" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.2">
@@ -14783,7 +14897,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I65" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.2">
@@ -14807,7 +14921,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I66" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.2">
@@ -14831,7 +14945,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I67" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.2">
@@ -14855,7 +14969,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I68" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.2">
@@ -14879,7 +14993,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I69" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.2">
@@ -14903,7 +15017,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I70" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.2">
@@ -14927,7 +15041,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I71" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.2">
@@ -14951,7 +15065,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I72" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.2">
@@ -14975,7 +15089,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I73" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.2">
@@ -14999,7 +15113,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I74" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.2">
@@ -15023,7 +15137,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I75" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.2">
@@ -15047,7 +15161,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I76" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.2">
@@ -15071,7 +15185,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I77" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.2">
@@ -15095,7 +15209,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I78" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.2">
@@ -15119,7 +15233,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I79" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.2">
@@ -15143,7 +15257,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="81" spans="4:9" x14ac:dyDescent="0.2">
@@ -15167,7 +15281,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I81" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="82" spans="4:9" x14ac:dyDescent="0.2">
@@ -15191,7 +15305,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I82" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="83" spans="4:9" x14ac:dyDescent="0.2">
@@ -15215,7 +15329,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I83" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="84" spans="4:9" x14ac:dyDescent="0.2">
@@ -15239,7 +15353,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I84" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="85" spans="4:9" x14ac:dyDescent="0.2">
@@ -15263,7 +15377,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I85" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="86" spans="4:9" x14ac:dyDescent="0.2">
@@ -15287,7 +15401,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I86" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="87" spans="4:9" x14ac:dyDescent="0.2">
@@ -15311,7 +15425,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I87" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="88" spans="4:9" x14ac:dyDescent="0.2">
@@ -15335,7 +15449,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I88" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="89" spans="4:9" x14ac:dyDescent="0.2">
@@ -15359,7 +15473,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I89" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="90" spans="4:9" x14ac:dyDescent="0.2">
@@ -15383,7 +15497,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I90" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="91" spans="4:9" x14ac:dyDescent="0.2">
@@ -15407,7 +15521,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I91" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="92" spans="4:9" x14ac:dyDescent="0.2">
@@ -15431,7 +15545,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I92" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="93" spans="4:9" x14ac:dyDescent="0.2">
@@ -15455,7 +15569,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I93" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="94" spans="4:9" x14ac:dyDescent="0.2">
@@ -15479,7 +15593,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I94" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="95" spans="4:9" x14ac:dyDescent="0.2">
@@ -15503,7 +15617,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I95" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="96" spans="4:9" x14ac:dyDescent="0.2">
@@ -15527,7 +15641,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I96" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
@@ -15551,7 +15665,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I97" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
@@ -15575,7 +15689,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I98" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
@@ -15599,7 +15713,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I99" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
@@ -15623,7 +15737,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I100" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
@@ -15647,7 +15761,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I101" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
@@ -15671,7 +15785,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I102" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
@@ -15695,7 +15809,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I103" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
@@ -15719,7 +15833,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I104" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
@@ -15743,7 +15857,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I105" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
@@ -15767,7 +15881,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I106" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
@@ -15791,7 +15905,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I107" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
@@ -15815,7 +15929,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I108" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
@@ -15839,7 +15953,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I109" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
@@ -15863,7 +15977,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I110" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
@@ -15887,7 +16001,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I111" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
@@ -15911,7 +16025,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I112" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="113" spans="4:9" x14ac:dyDescent="0.2">
@@ -15935,7 +16049,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I113" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="114" spans="4:9" x14ac:dyDescent="0.2">
@@ -15959,7 +16073,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I114" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="115" spans="4:9" x14ac:dyDescent="0.2">
@@ -15983,7 +16097,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I115" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="116" spans="4:9" x14ac:dyDescent="0.2">
@@ -16007,7 +16121,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I116" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="117" spans="4:9" x14ac:dyDescent="0.2">
@@ -16031,7 +16145,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I117" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="118" spans="4:9" x14ac:dyDescent="0.2">
@@ -16055,7 +16169,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I118" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="119" spans="4:9" x14ac:dyDescent="0.2">
@@ -16079,7 +16193,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I119" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="120" spans="4:9" x14ac:dyDescent="0.2">
@@ -16103,7 +16217,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I120" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="121" spans="4:9" x14ac:dyDescent="0.2">
@@ -16127,7 +16241,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I121" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="122" spans="4:9" x14ac:dyDescent="0.2">
@@ -16151,7 +16265,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I122" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="123" spans="4:9" x14ac:dyDescent="0.2">
@@ -16175,7 +16289,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I123" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="124" spans="4:9" x14ac:dyDescent="0.2">
@@ -16199,7 +16313,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I124" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="125" spans="4:9" x14ac:dyDescent="0.2">
@@ -16223,7 +16337,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I125" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -16247,7 +16361,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I126" s="165" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
@@ -16270,7 +16384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16743,7 +16857,7 @@
       </c>
       <c r="D14" s="120" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC3M#0001</v>
+        <v>_HKDYC3M#0002</v>
       </c>
       <c r="E14" s="95"/>
       <c r="F14" s="94"/>
@@ -17256,9 +17370,9 @@
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
         <v>41597</v>
       </c>
-      <c r="D27" s="101">
+      <c r="D27" s="101" t="e">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="E27" s="95"/>
       <c r="F27" s="94"/>
@@ -17295,11 +17409,11 @@
       <c r="B28" s="98"/>
       <c r="C28" s="100">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>47077</v>
-      </c>
-      <c r="D28" s="99">
+        <v>41962</v>
+      </c>
+      <c r="D28" s="99" t="e">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.65497637364458239</v>
+        <v>#NUM!</v>
       </c>
       <c r="E28" s="95"/>
       <c r="F28" s="94"/>
@@ -17338,8 +17452,8 @@
         <v>96</v>
       </c>
       <c r="D29" s="96" t="str">
-        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
+        <v>qlPiecewiseYieldCurveData - 1st instrument (maturity: March 19th, 2014) has an invalid quote</v>
       </c>
       <c r="E29" s="95"/>
       <c r="F29" s="94"/>

</xml_diff>